<commit_message>
Added taltech collab + ADAS experiments.
</commit_message>
<xml_diff>
--- a/R/progress.xlsx
+++ b/R/progress.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23716"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24102"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_ED130754D0C3BC56F02E5EEDF1B1A0EC2C7307B5" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7AEA4AC6-AC2E-4739-99CC-DB080C5E635E}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="11_ED130754D0C3BC56F02E5EEDF1B1A0EC2C7307B5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D52F4FB3-2841-4E34-9267-02E38E549AA4}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>block</t>
   </si>
@@ -38,9 +38,15 @@
     <t>coverage</t>
   </si>
   <si>
+    <t>User</t>
+  </si>
+  <si>
     <t>1S1</t>
   </si>
   <si>
+    <t>Anon</t>
+  </si>
+  <si>
     <t>1S2</t>
   </si>
   <si>
@@ -104,6 +110,9 @@
     <t>1S22</t>
   </si>
   <si>
+    <t>John</t>
+  </si>
+  <si>
     <t>1S23</t>
   </si>
   <si>
@@ -137,9 +146,15 @@
     <t>2S9</t>
   </si>
   <si>
+    <t>Ariane</t>
+  </si>
+  <si>
     <t>2S10</t>
   </si>
   <si>
+    <t>Jacob</t>
+  </si>
+  <si>
     <t>2S11</t>
   </si>
   <si>
@@ -164,9 +179,27 @@
     <t>1T1</t>
   </si>
   <si>
+    <t>Yara</t>
+  </si>
+  <si>
     <t>2T1</t>
   </si>
   <si>
+    <t>1X1</t>
+  </si>
+  <si>
+    <t>1X2</t>
+  </si>
+  <si>
+    <t>1X3</t>
+  </si>
+  <si>
+    <t>1X4</t>
+  </si>
+  <si>
+    <t>1X5</t>
+  </si>
+  <si>
     <t>1X6</t>
   </si>
   <si>
@@ -200,9 +233,6 @@
     <t>3MP1</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Team Member</t>
   </si>
   <si>
@@ -212,9 +242,6 @@
     <t>user2</t>
   </si>
   <si>
-    <t>Jacob</t>
-  </si>
-  <si>
     <t>user3</t>
   </si>
   <si>
@@ -224,9 +251,6 @@
     <t>user4</t>
   </si>
   <si>
-    <t>Yara</t>
-  </si>
-  <si>
     <t>user5</t>
   </si>
   <si>
@@ -234,9 +258,6 @@
   </si>
   <si>
     <t>user6</t>
-  </si>
-  <si>
-    <t>John</t>
   </si>
   <si>
     <t>user7</t>
@@ -258,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,8 +301,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,8 +335,26 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -310,21 +369,6 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -441,19 +485,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -475,10 +506,8 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -487,9 +516,7 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -500,20 +527,20 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -524,35 +551,37 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -562,41 +591,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
@@ -912,500 +992,727 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="23" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="19" t="b">
+      <c r="B2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="19" t="b">
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="19" t="b">
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="19" t="b">
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="19" t="b">
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="19" t="b">
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="19" t="b">
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="19" t="b">
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="19" t="b">
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="19" t="b">
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="19" t="b">
+      <c r="D12" s="24"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="19" t="b">
+      <c r="D13" s="24"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="19" t="b">
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="19" t="b">
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="19" t="b">
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="19" t="b">
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="19" t="b">
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="19" t="b">
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="19" t="b">
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="19" t="b">
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="19" t="b">
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="17" t="b">
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="24" t="s">
+      <c r="D25" s="24"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="11"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="24" t="s">
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="24" t="s">
+      <c r="B27" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="11"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="24" t="s">
+      <c r="B28" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="24" t="s">
+      <c r="B29" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="24" t="s">
+      <c r="B30" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="11"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="24" t="s">
+      <c r="B31" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="24" t="s">
+      <c r="B32" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="24" t="s">
+      <c r="B33" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="11"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="24" t="s">
+      <c r="B34" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="25" t="s">
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="12"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="24" t="s">
+      <c r="B35" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="11"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="24" t="s">
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="11"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="26" t="s">
+      <c r="B36" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="15"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="24" t="s">
+      <c r="B37" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="11"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="26" t="s">
+      <c r="B38" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="15"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="24" t="s">
+      <c r="B39" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="11"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="26" t="s">
+      <c r="B40" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="24" t="s">
+      <c r="B41" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="11"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="26" t="s">
+      <c r="B42" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C42" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="15"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="24" t="s">
+      <c r="B43" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="11"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="22" t="s">
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="23" t="s">
+      <c r="B44" s="12"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="23" t="s">
+      <c r="B45" s="36"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="24" t="s">
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="24" t="s">
+      <c r="B47" s="39"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="41"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="13"/>
-      <c r="C54" s="11"/>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="27" t="s">
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="2"/>
+      <c r="B49" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="35"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="46"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="44"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="46"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="46"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="44"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="46"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="44"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="46"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="44"/>
+      <c r="C57" s="45"/>
+      <c r="D57" s="46"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="48"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="51"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="48"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="51"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="53"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1416,7 +1723,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4215564F-F71D-491D-9B2A-B3A63BF30986}">
   <dimension ref="B2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1425,84 +1734,84 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>58</v>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="6"/>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>61</v>
+      <c r="B4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>63</v>
+      <c r="B5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>65</v>
+      <c r="B6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>67</v>
+      <c r="B7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>69</v>
+      <c r="B8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>71</v>
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="8"/>
+      <c r="B12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1510,9 +1819,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1727,16 +2039,13 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0C0C23E-F0F5-4EAB-AC5C-8BE9E5F48E1E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E214636A-0847-4F37-B132-F755F0C4B0DC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1744,5 +2053,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E214636A-0847-4F37-B132-F755F0C4B0DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0C0C23E-F0F5-4EAB-AC5C-8BE9E5F48E1E}"/>
 </file>
</xml_diff>